<commit_message>
Deploying to gh-pages from @ sorrychoe/covid19today@d439833b20b4d3d8d3a3bd7f16074eb66b2f6c1a 🚀
</commit_message>
<xml_diff>
--- a/reference/covid19.xlsx
+++ b/reference/covid19.xlsx
@@ -473,28 +473,28 @@
         </is>
       </c>
       <c r="C3">
-        <v>217403422</v>
+        <v>217408107</v>
       </c>
       <c r="D3">
-        <v>17947</v>
+        <v>22142</v>
       </c>
       <c r="E3">
-        <v>1546473</v>
+        <v>1546495</v>
       </c>
       <c r="F3">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="G3">
-        <v>201089197</v>
+        <v>201093712</v>
       </c>
       <c r="H3">
-        <v>8139</v>
+        <v>11705</v>
       </c>
       <c r="I3">
-        <v>14767752</v>
+        <v>14767900</v>
       </c>
       <c r="J3">
-        <v>15424</v>
+        <v>15409</v>
       </c>
     </row>
     <row r="4">
@@ -509,19 +509,25 @@
         </is>
       </c>
       <c r="C4">
-        <v>249316889</v>
+        <v>249318460</v>
+      </c>
+      <c r="D4">
+        <v>503</v>
       </c>
       <c r="E4">
-        <v>2060484</v>
+        <v>2060520</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
       </c>
       <c r="G4">
-        <v>245287445</v>
+        <v>245288281</v>
       </c>
       <c r="H4">
-        <v>3649</v>
+        <v>4404</v>
       </c>
       <c r="I4">
-        <v>1968960</v>
+        <v>1969659</v>
       </c>
       <c r="J4">
         <v>5797</v>
@@ -569,7 +575,10 @@
         </is>
       </c>
       <c r="C6">
-        <v>14323772</v>
+        <v>14323773</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
       </c>
       <c r="E6">
         <v>27858</v>
@@ -578,7 +587,7 @@
         <v>14150460</v>
       </c>
       <c r="I6">
-        <v>145454</v>
+        <v>145455</v>
       </c>
       <c r="J6">
         <v>86</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ sorrychoe/covid19today@9c9c0dff451bd6a8a1e5832a272bc0b40c17fb31 🚀
</commit_message>
<xml_diff>
--- a/reference/covid19.xlsx
+++ b/reference/covid19.xlsx
@@ -446,19 +446,19 @@
         </is>
       </c>
       <c r="C2">
-        <v>126695452</v>
+        <v>126698504</v>
       </c>
       <c r="E2">
-        <v>1633233</v>
+        <v>1633265</v>
       </c>
       <c r="G2">
-        <v>122569165</v>
+        <v>122584810</v>
       </c>
       <c r="I2">
-        <v>2493054</v>
+        <v>2480429</v>
       </c>
       <c r="J2">
-        <v>6220</v>
+        <v>6212</v>
       </c>
     </row>
     <row r="3">
@@ -473,28 +473,28 @@
         </is>
       </c>
       <c r="C3">
-        <v>217408107</v>
+        <v>217425850</v>
       </c>
       <c r="D3">
-        <v>22142</v>
+        <v>17533</v>
       </c>
       <c r="E3">
-        <v>1546495</v>
+        <v>1546499</v>
       </c>
       <c r="F3">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="G3">
-        <v>201093712</v>
+        <v>201115588</v>
       </c>
       <c r="H3">
-        <v>11705</v>
+        <v>21652</v>
       </c>
       <c r="I3">
-        <v>14767900</v>
+        <v>14763763</v>
       </c>
       <c r="J3">
-        <v>15409</v>
+        <v>15404</v>
       </c>
     </row>
     <row r="4">
@@ -509,28 +509,22 @@
         </is>
       </c>
       <c r="C4">
-        <v>249318460</v>
-      </c>
-      <c r="D4">
-        <v>503</v>
+        <v>249360306</v>
       </c>
       <c r="E4">
-        <v>2060520</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
+        <v>2061014</v>
       </c>
       <c r="G4">
-        <v>245288281</v>
+        <v>245331922</v>
       </c>
       <c r="H4">
-        <v>4404</v>
+        <v>4381</v>
       </c>
       <c r="I4">
-        <v>1969659</v>
+        <v>1967370</v>
       </c>
       <c r="J4">
-        <v>5797</v>
+        <v>5792</v>
       </c>
     </row>
     <row r="5">
@@ -545,22 +539,22 @@
         </is>
       </c>
       <c r="C5">
-        <v>68711068</v>
+        <v>68711939</v>
       </c>
       <c r="E5">
-        <v>1355880</v>
+        <v>1355891</v>
       </c>
       <c r="G5">
-        <v>66471120</v>
+        <v>66471658</v>
       </c>
       <c r="H5">
-        <v>229</v>
+        <v>246</v>
       </c>
       <c r="I5">
-        <v>884068</v>
+        <v>884390</v>
       </c>
       <c r="J5">
-        <v>10119</v>
+        <v>10123</v>
       </c>
     </row>
     <row r="6">
@@ -575,22 +569,19 @@
         </is>
       </c>
       <c r="C6">
-        <v>14323773</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
+        <v>14365172</v>
       </c>
       <c r="E6">
-        <v>27858</v>
+        <v>28077</v>
       </c>
       <c r="G6">
-        <v>14150460</v>
+        <v>14188517</v>
       </c>
       <c r="I6">
-        <v>145455</v>
+        <v>148578</v>
       </c>
       <c r="J6">
-        <v>86</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7">
@@ -605,16 +596,19 @@
         </is>
       </c>
       <c r="C7">
-        <v>12823412</v>
+        <v>12823515</v>
       </c>
       <c r="E7">
         <v>258765</v>
       </c>
       <c r="G7">
-        <v>12085348</v>
+        <v>12085476</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
       </c>
       <c r="I7">
-        <v>479299</v>
+        <v>479274</v>
       </c>
       <c r="J7">
         <v>548</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ sorrychoe/covid19today@8f235a589c1f5ff3dd7ce73757b8c1d7545d1e6f 🚀
</commit_message>
<xml_diff>
--- a/reference/covid19.xlsx
+++ b/reference/covid19.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,77 +360,47 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Country</t>
+          <t>Continent</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Continent</t>
+          <t>TotalCases</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>TotalCases</t>
+          <t>NewCases</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>NewCases</t>
+          <t>TotalDeaths</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>TotalDeaths</t>
+          <t>NewDeaths</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>NewDeaths</t>
+          <t>TotalRecovered</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>TotalRecovered</t>
+          <t>NewRecovered</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>NewRecovered</t>
+          <t>ActiveCases</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>ActiveCases</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
           <t>Critical</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Tot Cases/1M pop</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Deaths/1M pop</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>TotalTests</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Tests/1M pop</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Population</t>
         </is>
       </c>
     </row>
@@ -440,24 +410,19 @@
           <t>North America</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>North America</t>
-        </is>
-      </c>
-      <c r="C2">
-        <v>126698504</v>
-      </c>
-      <c r="E2">
-        <v>1633265</v>
-      </c>
-      <c r="G2">
-        <v>122584810</v>
+      <c r="B2">
+        <v>126699963</v>
+      </c>
+      <c r="D2">
+        <v>1633266</v>
+      </c>
+      <c r="F2">
+        <v>122586057</v>
+      </c>
+      <c r="H2">
+        <v>2480640</v>
       </c>
       <c r="I2">
-        <v>2480429</v>
-      </c>
-      <c r="J2">
         <v>6212</v>
       </c>
     </row>
@@ -467,34 +432,26 @@
           <t>Asia</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Asia</t>
-        </is>
+      <c r="B3">
+        <v>217430622</v>
       </c>
       <c r="C3">
-        <v>217425850</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>17533</v>
-      </c>
-      <c r="E3">
-        <v>1546499</v>
+        <v>1546531</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>201143899</v>
       </c>
       <c r="G3">
-        <v>201115588</v>
+        <v>23504</v>
       </c>
       <c r="H3">
-        <v>21652</v>
+        <v>14740192</v>
       </c>
       <c r="I3">
-        <v>14763763</v>
-      </c>
-      <c r="J3">
-        <v>15404</v>
+        <v>15363</v>
       </c>
     </row>
     <row r="4">
@@ -503,27 +460,22 @@
           <t>Europe</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Europe</t>
-        </is>
-      </c>
-      <c r="C4">
-        <v>249360306</v>
-      </c>
-      <c r="E4">
-        <v>2061014</v>
+      <c r="B4">
+        <v>249364068</v>
+      </c>
+      <c r="D4">
+        <v>2061022</v>
+      </c>
+      <c r="F4">
+        <v>245341050</v>
       </c>
       <c r="G4">
-        <v>245331922</v>
+        <v>5305</v>
       </c>
       <c r="H4">
-        <v>4381</v>
+        <v>1961996</v>
       </c>
       <c r="I4">
-        <v>1967370</v>
-      </c>
-      <c r="J4">
         <v>5792</v>
       </c>
     </row>
@@ -533,54 +485,41 @@
           <t>South America</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>South America</t>
-        </is>
-      </c>
-      <c r="C5">
-        <v>68711939</v>
-      </c>
-      <c r="E5">
+      <c r="B5">
+        <v>68711998</v>
+      </c>
+      <c r="D5">
         <v>1355891</v>
       </c>
-      <c r="G5">
-        <v>66471658</v>
+      <c r="F5">
+        <v>66471722</v>
       </c>
       <c r="H5">
-        <v>246</v>
+        <v>884385</v>
       </c>
       <c r="I5">
-        <v>884390</v>
-      </c>
-      <c r="J5">
         <v>10123</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Oceania</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
           <t>Australia/Oceania</t>
         </is>
       </c>
-      <c r="C6">
-        <v>14365172</v>
-      </c>
-      <c r="E6">
+      <c r="B6">
+        <v>14365175</v>
+      </c>
+      <c r="D6">
         <v>28077</v>
       </c>
-      <c r="G6">
+      <c r="F6">
         <v>14188517</v>
       </c>
+      <c r="H6">
+        <v>148581</v>
+      </c>
       <c r="I6">
-        <v>148578</v>
-      </c>
-      <c r="J6">
         <v>99</v>
       </c>
     </row>
@@ -590,44 +529,36 @@
           <t>Africa</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Africa</t>
-        </is>
-      </c>
-      <c r="C7">
-        <v>12823515</v>
-      </c>
-      <c r="E7">
+      <c r="B7">
+        <v>12823522</v>
+      </c>
+      <c r="D7">
         <v>258765</v>
       </c>
-      <c r="G7">
-        <v>12085476</v>
+      <c r="F7">
+        <v>12085479</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>479278</v>
       </c>
       <c r="I7">
-        <v>479274</v>
-      </c>
-      <c r="J7">
         <v>548</v>
       </c>
     </row>
     <row r="8">
-      <c r="C8">
+      <c r="B8">
         <v>721</v>
       </c>
-      <c r="E8">
+      <c r="D8">
         <v>15</v>
       </c>
-      <c r="G8">
+      <c r="F8">
         <v>706</v>
       </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
       <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ sorrychoe/covid19today@d3e56443830d7413be4737ece4cba6da31681b29 🚀
</commit_message>
<xml_diff>
--- a/reference/covid19.xlsx
+++ b/reference/covid19.xlsx
@@ -433,25 +433,28 @@
         </is>
       </c>
       <c r="B3">
-        <v>217430622</v>
+        <v>217433783</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>3162</v>
       </c>
       <c r="D3">
-        <v>1546531</v>
+        <v>1546556</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
       </c>
       <c r="F3">
-        <v>201143899</v>
+        <v>201147206</v>
       </c>
       <c r="G3">
-        <v>23504</v>
+        <v>26811</v>
       </c>
       <c r="H3">
-        <v>14740192</v>
+        <v>14740021</v>
       </c>
       <c r="I3">
-        <v>15363</v>
+        <v>15346</v>
       </c>
     </row>
     <row r="4">
@@ -461,19 +464,25 @@
         </is>
       </c>
       <c r="B4">
-        <v>249364068</v>
+        <v>249364590</v>
+      </c>
+      <c r="C4">
+        <v>189</v>
       </c>
       <c r="D4">
-        <v>2061022</v>
+        <v>2061026</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
       </c>
       <c r="F4">
-        <v>245341050</v>
+        <v>245341950</v>
       </c>
       <c r="G4">
-        <v>5305</v>
+        <v>5581</v>
       </c>
       <c r="H4">
-        <v>1961996</v>
+        <v>1961614</v>
       </c>
       <c r="I4">
         <v>5792</v>
@@ -514,10 +523,13 @@
         <v>28077</v>
       </c>
       <c r="F6">
-        <v>14188517</v>
+        <v>14188518</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>148581</v>
+        <v>148580</v>
       </c>
       <c r="I6">
         <v>99</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ sorrychoe/covid19today@aedddbe2493beee50db96325f07f30ade2172b04 🚀
</commit_message>
<xml_diff>
--- a/reference/covid19.xlsx
+++ b/reference/covid19.xlsx
@@ -411,19 +411,22 @@
         </is>
       </c>
       <c r="B2">
-        <v>126699963</v>
+        <v>126822971</v>
       </c>
       <c r="D2">
-        <v>1633266</v>
+        <v>1635327</v>
       </c>
       <c r="F2">
-        <v>122586057</v>
+        <v>122775364</v>
+      </c>
+      <c r="G2">
+        <v>4343</v>
       </c>
       <c r="H2">
-        <v>2480640</v>
+        <v>2412280</v>
       </c>
       <c r="I2">
-        <v>6212</v>
+        <v>6014</v>
       </c>
     </row>
     <row r="3">
@@ -433,28 +436,28 @@
         </is>
       </c>
       <c r="B3">
-        <v>217433783</v>
+        <v>217735242</v>
       </c>
       <c r="C3">
-        <v>3162</v>
+        <v>1220</v>
       </c>
       <c r="D3">
-        <v>1546556</v>
+        <v>1547009</v>
       </c>
       <c r="E3">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F3">
-        <v>201147206</v>
+        <v>201469871</v>
       </c>
       <c r="G3">
-        <v>26811</v>
+        <v>25229</v>
       </c>
       <c r="H3">
-        <v>14740021</v>
+        <v>14718362</v>
       </c>
       <c r="I3">
-        <v>15346</v>
+        <v>15191</v>
       </c>
     </row>
     <row r="4">
@@ -464,28 +467,28 @@
         </is>
       </c>
       <c r="B4">
-        <v>249364590</v>
+        <v>249540289</v>
       </c>
       <c r="C4">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="D4">
-        <v>2061026</v>
+        <v>2063821</v>
       </c>
       <c r="E4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>245341950</v>
+        <v>245545159</v>
       </c>
       <c r="G4">
-        <v>5581</v>
+        <v>3004</v>
       </c>
       <c r="H4">
-        <v>1961614</v>
+        <v>1931309</v>
       </c>
       <c r="I4">
-        <v>5792</v>
+        <v>5640</v>
       </c>
     </row>
     <row r="5">
@@ -495,19 +498,22 @@
         </is>
       </c>
       <c r="B5">
-        <v>68711998</v>
+        <v>68766612</v>
       </c>
       <c r="D5">
-        <v>1355891</v>
+        <v>1356746</v>
       </c>
       <c r="F5">
-        <v>66471722</v>
+        <v>66479577</v>
+      </c>
+      <c r="G5">
+        <v>511</v>
       </c>
       <c r="H5">
-        <v>884385</v>
+        <v>930289</v>
       </c>
       <c r="I5">
-        <v>10123</v>
+        <v>10104</v>
       </c>
     </row>
     <row r="6">
@@ -517,19 +523,16 @@
         </is>
       </c>
       <c r="B6">
-        <v>14365175</v>
+        <v>14458069</v>
       </c>
       <c r="D6">
-        <v>28077</v>
+        <v>28511</v>
       </c>
       <c r="F6">
-        <v>14188518</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
+        <v>14291244</v>
       </c>
       <c r="H6">
-        <v>148580</v>
+        <v>138314</v>
       </c>
       <c r="I6">
         <v>99</v>
@@ -542,16 +545,16 @@
         </is>
       </c>
       <c r="B7">
-        <v>12823522</v>
+        <v>12825765</v>
       </c>
       <c r="D7">
-        <v>258765</v>
+        <v>258782</v>
       </c>
       <c r="F7">
-        <v>12085479</v>
+        <v>12086419</v>
       </c>
       <c r="H7">
-        <v>479278</v>
+        <v>480564</v>
       </c>
       <c r="I7">
         <v>548</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ sorrychoe/covid19today@08c0e97e0b2efb38f5d9d4d8426506af2ca548a0 🚀
</commit_message>
<xml_diff>
--- a/reference/covid19.xlsx
+++ b/reference/covid19.xlsx
@@ -411,22 +411,22 @@
         </is>
       </c>
       <c r="B2">
-        <v>126822971</v>
+        <v>126947780</v>
       </c>
       <c r="D2">
-        <v>1635327</v>
+        <v>1636848</v>
       </c>
       <c r="F2">
-        <v>122775364</v>
+        <v>122930671</v>
       </c>
       <c r="G2">
-        <v>4343</v>
+        <v>517</v>
       </c>
       <c r="H2">
-        <v>2412280</v>
+        <v>2380261</v>
       </c>
       <c r="I2">
-        <v>6014</v>
+        <v>5953</v>
       </c>
     </row>
     <row r="3">
@@ -436,28 +436,28 @@
         </is>
       </c>
       <c r="B3">
-        <v>217735242</v>
+        <v>218123983</v>
       </c>
       <c r="C3">
-        <v>1220</v>
+        <v>669</v>
       </c>
       <c r="D3">
-        <v>1547009</v>
+        <v>1547511</v>
       </c>
       <c r="E3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F3">
-        <v>201469871</v>
+        <v>201785146</v>
       </c>
       <c r="G3">
-        <v>25229</v>
+        <v>1208</v>
       </c>
       <c r="H3">
-        <v>14718362</v>
+        <v>14791326</v>
       </c>
       <c r="I3">
-        <v>15191</v>
+        <v>15123</v>
       </c>
     </row>
     <row r="4">
@@ -467,28 +467,25 @@
         </is>
       </c>
       <c r="B4">
-        <v>249540289</v>
+        <v>249633231</v>
       </c>
       <c r="C4">
-        <v>173</v>
+        <v>257</v>
       </c>
       <c r="D4">
-        <v>2063821</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
+        <v>2065221</v>
       </c>
       <c r="F4">
-        <v>245545159</v>
+        <v>245715733</v>
       </c>
       <c r="G4">
-        <v>3004</v>
+        <v>1329</v>
       </c>
       <c r="H4">
-        <v>1931309</v>
+        <v>1852277</v>
       </c>
       <c r="I4">
-        <v>5640</v>
+        <v>5532</v>
       </c>
     </row>
     <row r="5">
@@ -498,22 +495,19 @@
         </is>
       </c>
       <c r="B5">
-        <v>68766612</v>
+        <v>68801962</v>
       </c>
       <c r="D5">
-        <v>1356746</v>
+        <v>1357193</v>
       </c>
       <c r="F5">
-        <v>66479577</v>
-      </c>
-      <c r="G5">
-        <v>511</v>
+        <v>66484069</v>
       </c>
       <c r="H5">
-        <v>930289</v>
+        <v>960700</v>
       </c>
       <c r="I5">
-        <v>10104</v>
+        <v>10100</v>
       </c>
     </row>
     <row r="6">
@@ -523,19 +517,19 @@
         </is>
       </c>
       <c r="B6">
-        <v>14458069</v>
+        <v>14521437</v>
       </c>
       <c r="D6">
-        <v>28511</v>
+        <v>28978</v>
       </c>
       <c r="F6">
-        <v>14291244</v>
+        <v>14355427</v>
       </c>
       <c r="H6">
-        <v>138314</v>
+        <v>137032</v>
       </c>
       <c r="I6">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7">
@@ -545,19 +539,19 @@
         </is>
       </c>
       <c r="B7">
-        <v>12825765</v>
+        <v>12829479</v>
       </c>
       <c r="D7">
-        <v>258782</v>
+        <v>258804</v>
       </c>
       <c r="F7">
-        <v>12086419</v>
+        <v>12087469</v>
       </c>
       <c r="H7">
-        <v>480564</v>
+        <v>483206</v>
       </c>
       <c r="I7">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ sorrychoe/covid19today@00135c9ffb276903a61aa47167095815779a3055 🚀
</commit_message>
<xml_diff>
--- a/reference/covid19.xlsx
+++ b/reference/covid19.xlsx
@@ -411,22 +411,22 @@
         </is>
       </c>
       <c r="B2">
-        <v>126947780</v>
+        <v>127514226</v>
       </c>
       <c r="D2">
-        <v>1636848</v>
+        <v>1642146</v>
       </c>
       <c r="F2">
-        <v>122930671</v>
+        <v>123371297</v>
       </c>
       <c r="G2">
-        <v>517</v>
+        <v>257</v>
       </c>
       <c r="H2">
-        <v>2380261</v>
+        <v>2500783</v>
       </c>
       <c r="I2">
-        <v>5953</v>
+        <v>6121</v>
       </c>
     </row>
     <row r="3">
@@ -436,28 +436,25 @@
         </is>
       </c>
       <c r="B3">
-        <v>218123983</v>
+        <v>220006270</v>
       </c>
       <c r="C3">
-        <v>669</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>1547511</v>
-      </c>
-      <c r="E3">
-        <v>4</v>
+        <v>1548725</v>
       </c>
       <c r="F3">
-        <v>201785146</v>
+        <v>203301226</v>
       </c>
       <c r="G3">
-        <v>1208</v>
+        <v>64155</v>
       </c>
       <c r="H3">
-        <v>14791326</v>
+        <v>15156319</v>
       </c>
       <c r="I3">
-        <v>15123</v>
+        <v>15135</v>
       </c>
     </row>
     <row r="4">
@@ -467,25 +464,22 @@
         </is>
       </c>
       <c r="B4">
-        <v>249633231</v>
-      </c>
-      <c r="C4">
-        <v>257</v>
+        <v>249785633</v>
       </c>
       <c r="D4">
-        <v>2065221</v>
+        <v>2069477</v>
       </c>
       <c r="F4">
-        <v>245715733</v>
+        <v>245928953</v>
       </c>
       <c r="G4">
-        <v>1329</v>
+        <v>580</v>
       </c>
       <c r="H4">
-        <v>1852277</v>
+        <v>1787203</v>
       </c>
       <c r="I4">
-        <v>5532</v>
+        <v>5443</v>
       </c>
     </row>
     <row r="5">
@@ -495,16 +489,16 @@
         </is>
       </c>
       <c r="B5">
-        <v>68801962</v>
+        <v>68933479</v>
       </c>
       <c r="D5">
-        <v>1357193</v>
+        <v>1359505</v>
       </c>
       <c r="F5">
-        <v>66484069</v>
+        <v>66510589</v>
       </c>
       <c r="H5">
-        <v>960700</v>
+        <v>1063385</v>
       </c>
       <c r="I5">
         <v>10100</v>
@@ -517,19 +511,19 @@
         </is>
       </c>
       <c r="B6">
-        <v>14521437</v>
+        <v>14608586</v>
       </c>
       <c r="D6">
-        <v>28978</v>
+        <v>30035</v>
       </c>
       <c r="F6">
-        <v>14355427</v>
+        <v>14469937</v>
       </c>
       <c r="H6">
-        <v>137032</v>
+        <v>108614</v>
       </c>
       <c r="I6">
-        <v>86</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7">
@@ -539,16 +533,16 @@
         </is>
       </c>
       <c r="B7">
-        <v>12829479</v>
+        <v>12836690</v>
       </c>
       <c r="D7">
-        <v>258804</v>
+        <v>258825</v>
       </c>
       <c r="F7">
-        <v>12087469</v>
+        <v>12088094</v>
       </c>
       <c r="H7">
-        <v>483206</v>
+        <v>489771</v>
       </c>
       <c r="I7">
         <v>547</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ sorrychoe/covid19today@da6a2b116f93465e736ec245d16f9ff0a7ab3c8c 🚀
</commit_message>
<xml_diff>
--- a/reference/covid19.xlsx
+++ b/reference/covid19.xlsx
@@ -360,208 +360,178 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Continent</t>
+          <t>TotalCases</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>TotalCases</t>
+          <t>NewCases</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>NewCases</t>
+          <t>TotalDeaths</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>TotalDeaths</t>
+          <t>NewDeaths</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>NewDeaths</t>
+          <t>TotalRecovered</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>TotalRecovered</t>
+          <t>NewRecovered</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>NewRecovered</t>
+          <t>ActiveCases</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>ActiveCases</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>TotalCasesPer1M</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>North America</t>
-        </is>
-      </c>
-      <c r="B2">
-        <v>127514226</v>
-      </c>
-      <c r="D2">
-        <v>1642146</v>
+      <c r="A2">
+        <v>131591034</v>
+      </c>
+      <c r="C2">
+        <v>1692184</v>
+      </c>
+      <c r="E2">
+        <v>127109905</v>
       </c>
       <c r="F2">
-        <v>123371297</v>
+        <v>665</v>
       </c>
       <c r="G2">
-        <v>257</v>
+        <v>2788945</v>
       </c>
       <c r="H2">
-        <v>2500783</v>
-      </c>
-      <c r="I2">
-        <v>6121</v>
+        <v>6709</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Asia</t>
-        </is>
-      </c>
-      <c r="B3">
-        <v>220006270</v>
+      <c r="A3">
+        <v>221465849</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1548725</v>
+        <v>1553248</v>
+      </c>
+      <c r="E3">
+        <v>205656562</v>
       </c>
       <c r="F3">
-        <v>203301226</v>
+        <v>308</v>
       </c>
       <c r="G3">
-        <v>64155</v>
+        <v>14256039</v>
       </c>
       <c r="H3">
-        <v>15156319</v>
-      </c>
-      <c r="I3">
-        <v>15135</v>
+        <v>14733</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Europe</t>
-        </is>
-      </c>
-      <c r="B4">
-        <v>249785633</v>
-      </c>
-      <c r="D4">
-        <v>2069477</v>
+      <c r="A4">
+        <v>253230160</v>
+      </c>
+      <c r="C4">
+        <v>2100520</v>
+      </c>
+      <c r="E4">
+        <v>248563147</v>
       </c>
       <c r="F4">
-        <v>245928953</v>
+        <v>5389</v>
       </c>
       <c r="G4">
-        <v>580</v>
+        <v>2566493</v>
       </c>
       <c r="H4">
-        <v>1787203</v>
-      </c>
-      <c r="I4">
-        <v>5443</v>
+        <v>4520</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>South America</t>
-        </is>
-      </c>
-      <c r="B5">
-        <v>68933479</v>
-      </c>
-      <c r="D5">
-        <v>1359505</v>
-      </c>
-      <c r="F5">
-        <v>66510589</v>
+      <c r="A5">
+        <v>69859756</v>
+      </c>
+      <c r="C5">
+        <v>1365807</v>
+      </c>
+      <c r="E5">
+        <v>66650237</v>
+      </c>
+      <c r="G5">
+        <v>1843712</v>
       </c>
       <c r="H5">
-        <v>1063385</v>
-      </c>
-      <c r="I5">
-        <v>10100</v>
+        <v>8953</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Australia/Oceania</t>
-        </is>
+      <c r="A6">
+        <v>14843156</v>
       </c>
       <c r="B6">
-        <v>14608586</v>
-      </c>
-      <c r="D6">
-        <v>30035</v>
-      </c>
-      <c r="F6">
-        <v>14469937</v>
+        <v>806</v>
+      </c>
+      <c r="C6">
+        <v>32737</v>
+      </c>
+      <c r="E6">
+        <v>14578860</v>
+      </c>
+      <c r="G6">
+        <v>231559</v>
       </c>
       <c r="H6">
-        <v>108614</v>
-      </c>
-      <c r="I6">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Africa</t>
-        </is>
-      </c>
-      <c r="B7">
-        <v>12836690</v>
-      </c>
-      <c r="D7">
-        <v>258825</v>
-      </c>
-      <c r="F7">
-        <v>12088094</v>
+      <c r="A7">
+        <v>12860287</v>
+      </c>
+      <c r="C7">
+        <v>258884</v>
+      </c>
+      <c r="E7">
+        <v>12090790</v>
+      </c>
+      <c r="G7">
+        <v>510613</v>
       </c>
       <c r="H7">
-        <v>489771</v>
-      </c>
-      <c r="I7">
-        <v>547</v>
+        <v>529</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8">
+      <c r="A8">
         <v>721</v>
       </c>
-      <c r="D8">
+      <c r="C8">
         <v>15</v>
       </c>
-      <c r="F8">
+      <c r="E8">
         <v>706</v>
       </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
       <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
         <v>0</v>
       </c>
     </row>

</xml_diff>